<commit_message>
doc update and quantile stat for plots
</commit_message>
<xml_diff>
--- a/fivecentplots/keywords.xlsx
+++ b/fivecentplots/keywords.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\fivecentplots\fivecentplots\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\fivecentplots\fivecentplots\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{F21DC55F-28F4-4D3C-B682-8D0B0807E384}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56467151-0903-490F-A987-DD1B385F8EBB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7800" tabRatio="862" firstSheet="9" activeTab="17" xr2:uid="{FB3948FF-1D23-4002-BA9B-90D3B8C27873}"/>
+    <workbookView xWindow="12015" yWindow="2130" windowWidth="19950" windowHeight="12750" tabRatio="862" firstSheet="7" activeTab="21" xr2:uid="{FB3948FF-1D23-4002-BA9B-90D3B8C27873}"/>
   </bookViews>
   <sheets>
     <sheet name="Mandatory" sheetId="11" r:id="rId1"/>
@@ -32,6 +32,10 @@
     <sheet name="Cbar" sheetId="19" r:id="rId17"/>
     <sheet name="Contour" sheetId="21" r:id="rId18"/>
     <sheet name="Heatmap" sheetId="20" r:id="rId19"/>
+    <sheet name="Stats" sheetId="22" r:id="rId20"/>
+    <sheet name="Gridlines" sheetId="23" r:id="rId21"/>
+    <sheet name="Data" sheetId="24" r:id="rId22"/>
+    <sheet name="Other" sheetId="25" r:id="rId23"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -43,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="536" uniqueCount="292">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="782" uniqueCount="417">
   <si>
     <t>Keyword</t>
   </si>
@@ -420,48 +424,6 @@
     <t>ax_size</t>
   </si>
   <si>
-    <t>:hh:`share_x`</t>
-  </si>
-  <si>
-    <t>:hh:`share_y`</t>
-  </si>
-  <si>
-    <t>:hh:`share_z`</t>
-  </si>
-  <si>
-    <t>:hh:`share_x2`</t>
-  </si>
-  <si>
-    <t>:hh:`share_y2`</t>
-  </si>
-  <si>
-    <t>:hh:`share_col`</t>
-  </si>
-  <si>
-    <t>:hh:`share_row`</t>
-  </si>
-  <si>
-    <t>:hh:`twin_x`</t>
-  </si>
-  <si>
-    <t>:hh:`twin_y`</t>
-  </si>
-  <si>
-    <t>:hh:`spines`</t>
-  </si>
-  <si>
-    <t>:hh:`spine_bottom`</t>
-  </si>
-  <si>
-    <t>:hh:`spine_left`</t>
-  </si>
-  <si>
-    <t>:hh:`spine_right`</t>
-  </si>
-  <si>
-    <t>:hh:`spine_top`</t>
-  </si>
-  <si>
     <t>hex color string</t>
   </si>
   <si>
@@ -645,9 +607,6 @@
     <t>padding in pixels from the top of the plot to the location of the fit eqn</t>
   </si>
   <si>
-    <t>:hh:`colors`</t>
-  </si>
-  <si>
     <t>hex color str or list of hex color strs</t>
   </si>
   <si>
@@ -660,9 +619,6 @@
     <t>`built-in color list &lt;styles.html#Built-in-color-list&gt;`_</t>
   </si>
   <si>
-    <t>:hh:`lines`</t>
-  </si>
-  <si>
     <t>toggle line visibility</t>
   </si>
   <si>
@@ -687,9 +643,6 @@
     <t>`Legend &lt;plot.html#Legend&gt;`_</t>
   </si>
   <si>
-    <t>:hh:`location`</t>
-  </si>
-  <si>
     <t>legend_marker_alpha</t>
   </si>
   <si>
@@ -882,9 +835,6 @@
     <t>box_stat_line_color</t>
   </si>
   <si>
-    <t>:hh:`dpi`</t>
-  </si>
-  <si>
     <t>toggle colorbar on/off for contour and heatmap plots</t>
   </si>
   <si>
@@ -903,35 +853,470 @@
     <t>inferno</t>
   </si>
   <si>
-    <t>:hh:`cbar`</t>
-  </si>
-  <si>
-    <t>:hh:`cmap`</t>
-  </si>
-  <si>
-    <t>:hh:`filled`</t>
-  </si>
-  <si>
     <t>Fill area between contour lines</t>
   </si>
   <si>
-    <t>:hh:`levels`</t>
-  </si>
-  <si>
     <t>Number of contour lines/levels to draw</t>
+  </si>
+  <si>
+    <t>stat</t>
+  </si>
+  <si>
+    <t>Add a line through a data set where each y-value represents a computed statistic of the data at a given x-value.  Options include:  'mean', 'median', 'std', 'q25' (25% quantile), etc</t>
+  </si>
+  <si>
+    <t>`Stat lines example &lt;plot.html#Stat-lines&gt;`_</t>
+  </si>
+  <si>
+    <t>stat_val</t>
+  </si>
+  <si>
+    <t>Column name to use instead of the given 'x' column for calculating the stat</t>
+  </si>
+  <si>
+    <t>conf_int</t>
+  </si>
+  <si>
+    <t>Add shading around a curve based on a given confidence interval from 0 to 1</t>
+  </si>
+  <si>
+    <t>` Confidence Intervals &lt;plot.html#Confidence-intervals&gt;`_</t>
+  </si>
+  <si>
+    <t>grid_major</t>
+  </si>
+  <si>
+    <t>` Major grid enabled/disabled &lt;ticks.html#Major-grid&gt;`_</t>
+  </si>
+  <si>
+    <t>grid_major_x</t>
+  </si>
+  <si>
+    <t>grid_major_y</t>
+  </si>
+  <si>
+    <t>grid_minor</t>
+  </si>
+  <si>
+    <t>grid_minor_x</t>
+  </si>
+  <si>
+    <t>grid_minor_y</t>
+  </si>
+  <si>
+    <t>Toggle major grid visibility for primary x axis</t>
+  </si>
+  <si>
+    <t>Toggle major grid visibility for primary x and y axes</t>
+  </si>
+  <si>
+    <t>Toggle major grid visibility for primary y axis</t>
+  </si>
+  <si>
+    <t>grid_major_x2</t>
+  </si>
+  <si>
+    <t>grid_major_y2</t>
+  </si>
+  <si>
+    <t>Toggle major grid visibility for secondary x axis</t>
+  </si>
+  <si>
+    <t>Toggle major grid visibility for secondary y axis</t>
+  </si>
+  <si>
+    <t>Toggle minor grid visibility for primary x and y axes</t>
+  </si>
+  <si>
+    <t>Toggle minor grid visibility for primary x axis</t>
+  </si>
+  <si>
+    <t>grid_minor_x2</t>
+  </si>
+  <si>
+    <t>Toggle minor grid visibility for secondary x axis</t>
+  </si>
+  <si>
+    <t>Toggle minor grid visibility for primary y axis</t>
+  </si>
+  <si>
+    <t>grid_minor_y2</t>
+  </si>
+  <si>
+    <t>Toggle minor grid visibility for secondary y axis</t>
+  </si>
+  <si>
+    <t>` Minor grid enabled/disabled &lt;ticks.html#Minor-grid&gt;`_</t>
+  </si>
+  <si>
+    <t>grid_major|minor_x|y|blank_color</t>
+  </si>
+  <si>
+    <t>grid_major|minor_x|y|blank_style</t>
+  </si>
+  <si>
+    <t>grid_major|minor_x|y|blank_width</t>
+  </si>
+  <si>
+    <t>Grid line color</t>
+  </si>
+  <si>
+    <t>Grid line style (follows matplotlib standards: '-', '--', etc)</t>
+  </si>
+  <si>
+    <t>Grid line width</t>
+  </si>
+  <si>
+    <t>data_labels</t>
+  </si>
+  <si>
+    <t>cell_size</t>
+  </si>
+  <si>
+    <t>`basic heatmap &lt;heatmap.html#No-data-labels&gt;`_</t>
+  </si>
+  <si>
+    <t>width of a heatmap cell</t>
+  </si>
+  <si>
+    <t>`cell size &lt;heatmap.html#Cell-size&gt;`_</t>
+  </si>
+  <si>
+    <t>enable/disable value labels on the heatmap cells</t>
+  </si>
+  <si>
+    <t>`data labels &lt;heatmap.html#With-data-labels&gt;`_</t>
+  </si>
+  <si>
+    <t>heatmap_font_xxx</t>
+  </si>
+  <si>
+    <t>various</t>
+  </si>
+  <si>
+    <t>data label fonts are controlled by standard font attributes with the prefix "heatmap_"</t>
+  </si>
+  <si>
+    <t>Various</t>
+  </si>
+  <si>
+    <t>show</t>
+  </si>
+  <si>
+    <t>inline</t>
+  </si>
+  <si>
+    <t>save</t>
+  </si>
+  <si>
+    <t>return_filename</t>
+  </si>
+  <si>
+    <t>filepath</t>
+  </si>
+  <si>
+    <t>print_filename</t>
+  </si>
+  <si>
+    <t>filename</t>
+  </si>
+  <si>
+    <t>save_ext</t>
+  </si>
+  <si>
+    <t>row</t>
+  </si>
+  <si>
+    <t>col</t>
+  </si>
+  <si>
+    <t>Open the **saved** plot (this is not the same as show in matplotlib)</t>
+  </si>
+  <si>
+    <t>Display the plot inline (in a jupyter notebook, using the matplotlib show command, etc)</t>
+  </si>
+  <si>
+    <t>Save the image</t>
+  </si>
+  <si>
+    <t>Return only the filename of the saved plot but not the plot itself</t>
+  </si>
+  <si>
+    <t>Directory in which the plot should be saved</t>
+  </si>
+  <si>
+    <t>Current directory</t>
+  </si>
+  <si>
+    <t>Print the filename and return the plot</t>
+  </si>
+  <si>
+    <t>Name of the saved plot</t>
+  </si>
+  <si>
+    <t>File extension for the saved plot</t>
+  </si>
+  <si>
+    <t>png</t>
+  </si>
+  <si>
+    <t>Built automatically based on plot conditions</t>
+  </si>
+  <si>
+    <t>dpi`</t>
+  </si>
+  <si>
+    <t>colors`</t>
+  </si>
+  <si>
+    <t>lines`</t>
+  </si>
+  <si>
+    <t>share_x</t>
+  </si>
+  <si>
+    <t>share_y</t>
+  </si>
+  <si>
+    <t>share_z</t>
+  </si>
+  <si>
+    <t>share_x2</t>
+  </si>
+  <si>
+    <t>share_y2</t>
+  </si>
+  <si>
+    <t>share_col</t>
+  </si>
+  <si>
+    <t>share_row</t>
+  </si>
+  <si>
+    <t>spines</t>
+  </si>
+  <si>
+    <t>spine_bottom</t>
+  </si>
+  <si>
+    <t>spine_left</t>
+  </si>
+  <si>
+    <t>spine_right</t>
+  </si>
+  <si>
+    <t>spine_top</t>
+  </si>
+  <si>
+    <t>twin_x</t>
+  </si>
+  <si>
+    <t>twin_y</t>
+  </si>
+  <si>
+    <t>location</t>
+  </si>
+  <si>
+    <t>cbar</t>
+  </si>
+  <si>
+    <t>filled</t>
+  </si>
+  <si>
+    <t>levels</t>
+  </si>
+  <si>
+    <t>auto_scale</t>
+  </si>
+  <si>
+    <t>fit_range_x</t>
+  </si>
+  <si>
+    <t>fit_range_y</t>
+  </si>
+  <si>
+    <t>list</t>
+  </si>
+  <si>
+    <t>compute the fit only over a given range of x-values</t>
+  </si>
+  <si>
+    <t>compute the fit only over a given range of y-values</t>
+  </si>
+  <si>
+    <t>`third example here &lt;plot.html#Curve-fitting&gt;`_</t>
+  </si>
+  <si>
+    <t>wrap</t>
+  </si>
+  <si>
+    <t>name of DataFrame column to use for column-based subplots</t>
+  </si>
+  <si>
+    <t>name of DataFrame column to use for row-based subplots</t>
+  </si>
+  <si>
+    <t>str|list</t>
+  </si>
+  <si>
+    <t>name or list of names of DataFrame columns for wrap-type subplots</t>
+  </si>
+  <si>
+    <t>trans_x</t>
+  </si>
+  <si>
+    <t>trans_x2</t>
+  </si>
+  <si>
+    <t>trans_y</t>
+  </si>
+  <si>
+    <t>trans_y2</t>
+  </si>
+  <si>
+    <t>trans_z</t>
+  </si>
+  <si>
+    <t>xmin</t>
+  </si>
+  <si>
+    <t>x2min</t>
+  </si>
+  <si>
+    <t>xmax</t>
+  </si>
+  <si>
+    <t>x2max</t>
+  </si>
+  <si>
+    <t>ymin</t>
+  </si>
+  <si>
+    <t>y2min</t>
+  </si>
+  <si>
+    <t>ymax</t>
+  </si>
+  <si>
+    <t>y2max</t>
+  </si>
+  <si>
+    <t>float|list of floats|None</t>
+  </si>
+  <si>
+    <t>minimum x-values; can use a list for each subplot</t>
+  </si>
+  <si>
+    <t>minimum y-values; can use a list for each subplot</t>
+  </si>
+  <si>
+    <t>maximum x-values; can use a list for each subplot</t>
+  </si>
+  <si>
+    <t>minimum y-values for secondary axis; can use a list for each subplot</t>
+  </si>
+  <si>
+    <t>maximum x-values for secondary axis; can use a list for each subplot</t>
+  </si>
+  <si>
+    <t>maximum y-values for secondary axis; can use a list for each subplot</t>
+  </si>
+  <si>
+    <t>maximum y-values; can use a list for each subplot</t>
+  </si>
+  <si>
+    <t>`primary axis &lt;ranges.html#Primary-axes-only&gt;`_</t>
+  </si>
+  <si>
+    <t>`secondary axis &lt;ranges.html#Secondary-y-axis&gt;`_</t>
+  </si>
+  <si>
+    <t>filter</t>
+  </si>
+  <si>
+    <t>ncol</t>
+  </si>
+  <si>
+    <t>fig_groups</t>
+  </si>
+  <si>
+    <t xml:space="preserve">enable/disable auto-scaling feature for one-side range </t>
+  </si>
+  <si>
+    <t>specification; not allowed for heatmap or histogram</t>
+  </si>
+  <si>
+    <t>`auto-scale &lt;ranges.html#Primary-axes-only&gt;`_</t>
+  </si>
+  <si>
+    <t>`column plot &lt;plot.html#Column-plot&gt;`_</t>
+  </si>
+  <si>
+    <t>str|list of str</t>
+  </si>
+  <si>
+    <t>DataFrame column(s) to use for figure-level grouping</t>
+  </si>
+  <si>
+    <t>`figure plots &lt;grouping.html#figure-plots&gt;`_</t>
+  </si>
+  <si>
+    <t>string-based DataFrame filter (similar to query in pandas)</t>
+  </si>
+  <si>
+    <t>see most plot examples</t>
+  </si>
+  <si>
+    <t>specify the number of columns in a wrap plot</t>
+  </si>
+  <si>
+    <t>try to make square grid</t>
+  </si>
+  <si>
+    <t>`compare two cases &lt;grouping.html?highlight=ncol#By-unique-values&gt;`_</t>
+  </si>
+  <si>
+    <t>`row plot &lt;plot.html#Row-plot&gt;`_</t>
+  </si>
+  <si>
+    <t>`axis sharing &lt;ranges.html#Axes-sharing&gt;`_</t>
+  </si>
+  <si>
+    <t>str|None</t>
+  </si>
+  <si>
+    <t>apply an axis transformation to a given axis</t>
+  </si>
+  <si>
+    <t>options: 'abs', 'negative' or 'neg', 'nq' (normal quantile)</t>
+  </si>
+  <si>
+    <t>inverse' or 'inv', ('pow', int), 'flip'</t>
+  </si>
+  <si>
+    <t>same as ``trans_x``</t>
+  </si>
+  <si>
+    <t>`wrap plot &lt;plot.html#Wrap-plot&gt;`_</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF333333"/>
+      <name val="Courier New"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -954,7 +1339,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -975,13 +1360,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1299,7 +1690,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1425,16 +1816,16 @@
         <v>19</v>
       </c>
       <c r="B2" t="s">
-        <v>185</v>
+        <v>171</v>
       </c>
       <c r="C2" t="s">
-        <v>207</v>
+        <v>191</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="8" t="s">
-        <v>208</v>
+      <c r="E2" s="9" t="s">
+        <v>192</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -1445,12 +1836,12 @@
         <v>64</v>
       </c>
       <c r="C3" t="s">
-        <v>209</v>
+        <v>193</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="E3" s="8"/>
+        <v>194</v>
+      </c>
+      <c r="E3" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1496,180 +1887,180 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>211</v>
+        <v>195</v>
       </c>
       <c r="B2" t="s">
         <v>64</v>
       </c>
       <c r="C2" t="s">
+        <v>196</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
+        <v>355</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>207</v>
+      </c>
+      <c r="C3" t="s">
+        <v>202</v>
+      </c>
+      <c r="D3" s="10">
+        <v>0</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="9"/>
+      <c r="B4" s="9"/>
+      <c r="C4" t="s">
+        <v>205</v>
+      </c>
+      <c r="D4" s="10"/>
+      <c r="E4" s="9"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="9"/>
+      <c r="B5" s="9"/>
+      <c r="C5" t="s">
+        <v>203</v>
+      </c>
+      <c r="D5" s="10"/>
+      <c r="E5" s="9"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="9"/>
+      <c r="B6" s="9"/>
+      <c r="C6" t="s">
+        <v>204</v>
+      </c>
+      <c r="D6" s="10"/>
+      <c r="E6" s="9"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="9"/>
+      <c r="B7" s="9"/>
+      <c r="C7" t="s">
+        <v>206</v>
+      </c>
+      <c r="D7" s="10"/>
+      <c r="E7" s="9"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="9"/>
+      <c r="B8" s="9"/>
+      <c r="C8" t="s">
+        <v>208</v>
+      </c>
+      <c r="D8" s="10"/>
+      <c r="E8" s="9"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="9"/>
+      <c r="B9" s="9"/>
+      <c r="C9" t="s">
+        <v>210</v>
+      </c>
+      <c r="D9" s="10"/>
+      <c r="E9" s="9"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="9"/>
+      <c r="B10" s="9"/>
+      <c r="C10" t="s">
+        <v>211</v>
+      </c>
+      <c r="D10" s="10"/>
+      <c r="E10" s="9"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="9"/>
+      <c r="B11" s="9"/>
+      <c r="C11" t="s">
         <v>212</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="D11" s="10"/>
+      <c r="E11" s="9"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="9"/>
+      <c r="B12" s="9"/>
+      <c r="C12" t="s">
+        <v>209</v>
+      </c>
+      <c r="D12" s="10"/>
+      <c r="E12" s="9"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="9"/>
+      <c r="B13" s="9"/>
+      <c r="C13" t="s">
         <v>213</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
+      <c r="D13" s="10"/>
+      <c r="E13" s="9"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="9"/>
+      <c r="B14" s="9"/>
+      <c r="C14" t="s">
         <v>214</v>
       </c>
-      <c r="B3" s="8" t="s">
-        <v>224</v>
-      </c>
-      <c r="C3" t="s">
-        <v>219</v>
-      </c>
-      <c r="D3" s="9">
-        <v>0</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="8"/>
-      <c r="B4" s="8"/>
-      <c r="C4" t="s">
-        <v>222</v>
-      </c>
-      <c r="D4" s="9"/>
-      <c r="E4" s="8"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="8"/>
-      <c r="B5" s="8"/>
-      <c r="C5" t="s">
-        <v>220</v>
-      </c>
-      <c r="D5" s="9"/>
-      <c r="E5" s="8"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="8"/>
-      <c r="B6" s="8"/>
-      <c r="C6" t="s">
-        <v>221</v>
-      </c>
-      <c r="D6" s="9"/>
-      <c r="E6" s="8"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="8"/>
-      <c r="B7" s="8"/>
-      <c r="C7" t="s">
-        <v>223</v>
-      </c>
-      <c r="D7" s="9"/>
-      <c r="E7" s="8"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="8"/>
-      <c r="B8" s="8"/>
-      <c r="C8" t="s">
-        <v>225</v>
-      </c>
-      <c r="D8" s="9"/>
-      <c r="E8" s="8"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="8"/>
-      <c r="B9" s="8"/>
-      <c r="C9" t="s">
-        <v>227</v>
-      </c>
-      <c r="D9" s="9"/>
-      <c r="E9" s="8"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="8"/>
-      <c r="B10" s="8"/>
-      <c r="C10" t="s">
-        <v>228</v>
-      </c>
-      <c r="D10" s="9"/>
-      <c r="E10" s="8"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="8"/>
-      <c r="B11" s="8"/>
-      <c r="C11" t="s">
-        <v>229</v>
-      </c>
-      <c r="D11" s="9"/>
-      <c r="E11" s="8"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="8"/>
-      <c r="B12" s="8"/>
-      <c r="C12" t="s">
-        <v>226</v>
-      </c>
-      <c r="D12" s="9"/>
-      <c r="E12" s="8"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="8"/>
-      <c r="B13" s="8"/>
-      <c r="C13" t="s">
-        <v>230</v>
-      </c>
-      <c r="D13" s="9"/>
-      <c r="E13" s="8"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="8"/>
-      <c r="B14" s="8"/>
-      <c r="C14" t="s">
-        <v>231</v>
-      </c>
-      <c r="D14" s="9"/>
-      <c r="E14" s="8"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="9"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
-        <v>215</v>
+        <v>198</v>
       </c>
       <c r="B15" t="s">
         <v>63</v>
       </c>
       <c r="C15" t="s">
-        <v>232</v>
+        <v>215</v>
       </c>
       <c r="D15">
         <v>1</v>
       </c>
       <c r="E15" t="s">
-        <v>233</v>
+        <v>216</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
-        <v>216</v>
+        <v>199</v>
       </c>
       <c r="B16" t="s">
         <v>63</v>
       </c>
       <c r="C16" t="s">
-        <v>234</v>
+        <v>217</v>
       </c>
       <c r="D16" t="s">
-        <v>235</v>
+        <v>218</v>
       </c>
       <c r="E16" t="s">
-        <v>187</v>
+        <v>173</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
-        <v>217</v>
+        <v>200</v>
       </c>
       <c r="B17" t="s">
         <v>62</v>
       </c>
       <c r="C17" t="s">
-        <v>236</v>
+        <v>219</v>
       </c>
       <c r="D17" s="3">
         <v>1</v>
@@ -1680,16 +2071,16 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
-        <v>218</v>
+        <v>201</v>
       </c>
       <c r="B18" t="s">
         <v>64</v>
       </c>
       <c r="C18" t="s">
-        <v>237</v>
+        <v>220</v>
       </c>
       <c r="D18" t="s">
-        <v>238</v>
+        <v>221</v>
       </c>
       <c r="E18" t="s">
         <v>30</v>
@@ -1753,7 +2144,7 @@
       <c r="D2" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="9" t="s">
         <v>91</v>
       </c>
     </row>
@@ -1770,7 +2161,7 @@
       <c r="D3" t="s">
         <v>89</v>
       </c>
-      <c r="E3" s="8"/>
+      <c r="E3" s="9"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -1785,7 +2176,7 @@
       <c r="D4" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="8"/>
+      <c r="E4" s="9"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -1800,7 +2191,7 @@
       <c r="D5" t="s">
         <v>90</v>
       </c>
-      <c r="E5" s="8"/>
+      <c r="E5" s="9"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -1815,7 +2206,7 @@
       <c r="D6" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="E6" s="8"/>
+      <c r="E6" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1868,7 +2259,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>274</v>
+        <v>257</v>
       </c>
       <c r="B3" t="s">
         <v>64</v>
@@ -1942,7 +2333,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>278</v>
+        <v>261</v>
       </c>
       <c r="B4" t="s">
         <v>64</v>
@@ -2002,7 +2393,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>275</v>
+        <v>258</v>
       </c>
       <c r="B3" t="s">
         <v>64</v>
@@ -2016,7 +2407,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>276</v>
+        <v>259</v>
       </c>
       <c r="B4" t="s">
         <v>64</v>
@@ -2030,7 +2421,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>277</v>
+        <v>260</v>
       </c>
       <c r="B5" t="s">
         <v>64</v>
@@ -2080,177 +2471,177 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
-        <v>253</v>
+      <c r="A2" s="9" t="s">
+        <v>236</v>
       </c>
       <c r="B2" t="s">
-        <v>239</v>
-      </c>
-      <c r="C2" s="8" t="s">
+        <v>222</v>
+      </c>
+      <c r="C2" s="9" t="s">
         <v>62</v>
       </c>
       <c r="D2" t="s">
-        <v>259</v>
+        <v>242</v>
       </c>
       <c r="E2">
         <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="8"/>
+      <c r="A3" s="9"/>
       <c r="B3" t="s">
-        <v>240</v>
-      </c>
-      <c r="C3" s="8"/>
+        <v>223</v>
+      </c>
+      <c r="C3" s="9"/>
       <c r="D3" t="s">
-        <v>260</v>
+        <v>243</v>
       </c>
       <c r="E3">
         <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="8"/>
+      <c r="A4" s="9"/>
       <c r="B4" t="s">
-        <v>241</v>
-      </c>
-      <c r="C4" s="8"/>
+        <v>224</v>
+      </c>
+      <c r="C4" s="9"/>
       <c r="D4" t="s">
-        <v>261</v>
+        <v>244</v>
       </c>
       <c r="E4">
         <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="8"/>
+      <c r="A5" s="9"/>
       <c r="B5" t="s">
-        <v>242</v>
-      </c>
-      <c r="C5" s="8"/>
+        <v>225</v>
+      </c>
+      <c r="C5" s="9"/>
       <c r="D5" t="s">
-        <v>262</v>
+        <v>245</v>
       </c>
       <c r="E5">
         <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
-        <v>254</v>
+      <c r="A6" s="9" t="s">
+        <v>237</v>
       </c>
       <c r="B6" t="s">
-        <v>243</v>
-      </c>
-      <c r="C6" s="8"/>
+        <v>226</v>
+      </c>
+      <c r="C6" s="9"/>
       <c r="D6" t="s">
-        <v>263</v>
+        <v>246</v>
       </c>
       <c r="E6">
         <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="8"/>
+      <c r="A7" s="9"/>
       <c r="B7" t="s">
-        <v>244</v>
-      </c>
-      <c r="C7" s="8"/>
+        <v>227</v>
+      </c>
+      <c r="C7" s="9"/>
       <c r="D7" t="s">
-        <v>264</v>
+        <v>247</v>
       </c>
       <c r="E7">
         <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="8"/>
+      <c r="A8" s="9"/>
       <c r="B8" t="s">
-        <v>245</v>
-      </c>
-      <c r="C8" s="8"/>
+        <v>228</v>
+      </c>
+      <c r="C8" s="9"/>
       <c r="D8" t="s">
-        <v>271</v>
+        <v>254</v>
       </c>
       <c r="E8">
         <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="8"/>
+      <c r="A9" s="9"/>
       <c r="B9" t="s">
-        <v>255</v>
-      </c>
-      <c r="C9" s="8"/>
+        <v>238</v>
+      </c>
+      <c r="C9" s="9"/>
       <c r="D9" t="s">
-        <v>265</v>
+        <v>248</v>
       </c>
       <c r="E9">
         <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="s">
-        <v>256</v>
+      <c r="A10" s="9" t="s">
+        <v>239</v>
       </c>
       <c r="B10" t="s">
-        <v>246</v>
-      </c>
-      <c r="C10" s="8"/>
+        <v>229</v>
+      </c>
+      <c r="C10" s="9"/>
       <c r="D10" t="s">
-        <v>266</v>
+        <v>249</v>
       </c>
       <c r="E10">
         <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="8"/>
+      <c r="A11" s="9"/>
       <c r="B11" t="s">
-        <v>247</v>
-      </c>
-      <c r="C11" s="8"/>
+        <v>230</v>
+      </c>
+      <c r="C11" s="9"/>
       <c r="D11" t="s">
-        <v>267</v>
+        <v>250</v>
       </c>
       <c r="E11">
         <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="8"/>
+      <c r="A12" s="9"/>
       <c r="B12" t="s">
-        <v>248</v>
-      </c>
-      <c r="C12" s="8"/>
+        <v>231</v>
+      </c>
+      <c r="C12" s="9"/>
       <c r="D12" t="s">
-        <v>268</v>
+        <v>251</v>
       </c>
       <c r="E12">
         <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="8"/>
+      <c r="A13" s="9"/>
       <c r="B13" t="s">
-        <v>249</v>
-      </c>
-      <c r="C13" s="8"/>
+        <v>232</v>
+      </c>
+      <c r="C13" s="9"/>
       <c r="D13" t="s">
-        <v>269</v>
+        <v>252</v>
       </c>
       <c r="E13">
         <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="8"/>
+      <c r="A14" s="9"/>
       <c r="B14" t="s">
-        <v>250</v>
-      </c>
-      <c r="C14" s="8"/>
+        <v>233</v>
+      </c>
+      <c r="C14" s="9"/>
       <c r="D14" t="s">
-        <v>270</v>
+        <v>253</v>
       </c>
       <c r="E14">
         <v>30</v>
@@ -2258,14 +2649,14 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>257</v>
+        <v>240</v>
       </c>
       <c r="B15" t="s">
-        <v>251</v>
-      </c>
-      <c r="C15" s="8"/>
+        <v>234</v>
+      </c>
+      <c r="C15" s="9"/>
       <c r="D15" t="s">
-        <v>272</v>
+        <v>255</v>
       </c>
       <c r="E15">
         <v>10</v>
@@ -2273,14 +2664,14 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>258</v>
+        <v>241</v>
       </c>
       <c r="B16" t="s">
-        <v>252</v>
-      </c>
-      <c r="C16" s="8"/>
+        <v>235</v>
+      </c>
+      <c r="C16" s="9"/>
       <c r="D16" t="s">
-        <v>273</v>
+        <v>256</v>
       </c>
       <c r="E16">
         <v>10</v>
@@ -2329,19 +2720,19 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>286</v>
+        <v>356</v>
       </c>
       <c r="B2" t="s">
         <v>65</v>
       </c>
       <c r="C2" t="s">
-        <v>280</v>
+        <v>262</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="E2" s="10" t="s">
-        <v>282</v>
+      <c r="E2" s="8" t="s">
+        <v>264</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -2352,12 +2743,12 @@
         <v>62</v>
       </c>
       <c r="C3" t="s">
-        <v>281</v>
+        <v>263</v>
       </c>
       <c r="D3" s="3">
         <v>30</v>
       </c>
-      <c r="E3" s="10"/>
+      <c r="E3" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2368,8 +2759,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DF9DEB0-6665-4538-AF49-F67F1AF6D966}">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2393,45 +2784,45 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>287</v>
+        <v>265</v>
       </c>
       <c r="B2" t="s">
         <v>64</v>
       </c>
       <c r="C2" t="s">
-        <v>284</v>
+        <v>266</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>285</v>
-      </c>
-      <c r="E2" s="10" t="s">
-        <v>282</v>
+        <v>267</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>264</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>288</v>
+        <v>357</v>
       </c>
       <c r="B3" t="s">
         <v>65</v>
       </c>
       <c r="C3" t="s">
-        <v>289</v>
+        <v>268</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="E3" s="10"/>
+      <c r="E3" s="8"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>290</v>
+        <v>358</v>
       </c>
       <c r="B4" t="s">
         <v>62</v>
       </c>
       <c r="C4" t="s">
-        <v>291</v>
+        <v>269</v>
       </c>
       <c r="D4">
         <v>20</v>
@@ -2444,13 +2835,20 @@
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB8856DC-C126-4FEE-B018-443AE2EE34DC}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="A1:E3"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="48.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="47" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -2470,36 +2868,72 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>283</v>
+      <c r="A2" s="12" t="s">
+        <v>307</v>
       </c>
       <c r="B2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C2" t="s">
-        <v>280</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="E2" s="10" t="s">
-        <v>282</v>
+        <v>309</v>
+      </c>
+      <c r="D2" s="3">
+        <v>60</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>310</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>23</v>
+        <v>265</v>
       </c>
       <c r="B3" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="C3" t="s">
-        <v>281</v>
-      </c>
-      <c r="D3" s="3">
-        <v>30</v>
-      </c>
-      <c r="E3" s="10"/>
+        <v>262</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>306</v>
+      </c>
+      <c r="B4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C4" t="s">
+        <v>311</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>313</v>
+      </c>
+      <c r="B5" t="s">
+        <v>314</v>
+      </c>
+      <c r="C5" t="s">
+        <v>315</v>
+      </c>
+      <c r="D5" t="s">
+        <v>316</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>30</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2538,7 +2972,7 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="9" t="s">
         <v>47</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -2555,7 +2989,7 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="8"/>
+      <c r="A3" s="9"/>
       <c r="B3" s="1" t="s">
         <v>64</v>
       </c>
@@ -2570,7 +3004,7 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="9" t="s">
         <v>48</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -2587,7 +3021,7 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="8"/>
+      <c r="A5" s="9"/>
       <c r="B5" s="1" t="s">
         <v>63</v>
       </c>
@@ -2602,7 +3036,7 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="8"/>
+      <c r="A6" s="9"/>
       <c r="B6" s="1" t="s">
         <v>64</v>
       </c>
@@ -2617,7 +3051,7 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="9" t="s">
         <v>49</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -2634,7 +3068,7 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="8"/>
+      <c r="A8" s="9"/>
       <c r="B8" s="1" t="s">
         <v>64</v>
       </c>
@@ -2649,7 +3083,7 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="8"/>
+      <c r="A9" s="9"/>
       <c r="B9" s="1" t="s">
         <v>63</v>
       </c>
@@ -2664,7 +3098,7 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="8"/>
+      <c r="A10" s="9"/>
       <c r="B10" s="1" t="s">
         <v>64</v>
       </c>
@@ -2679,7 +3113,7 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="8"/>
+      <c r="A11" s="9"/>
       <c r="B11" s="1" t="s">
         <v>64</v>
       </c>
@@ -2694,7 +3128,7 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="8" t="s">
+      <c r="A12" s="9" t="s">
         <v>54</v>
       </c>
       <c r="B12" s="1" t="s">
@@ -2711,7 +3145,7 @@
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="8"/>
+      <c r="A13" s="9"/>
       <c r="B13" s="1" t="s">
         <v>64</v>
       </c>
@@ -2726,7 +3160,7 @@
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="8"/>
+      <c r="A14" s="9"/>
       <c r="B14" s="1" t="s">
         <v>64</v>
       </c>
@@ -2741,7 +3175,7 @@
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="8"/>
+      <c r="A15" s="9"/>
       <c r="B15" s="2" t="s">
         <v>63</v>
       </c>
@@ -2756,7 +3190,7 @@
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="8" t="s">
+      <c r="A16" s="9" t="s">
         <v>55</v>
       </c>
       <c r="B16" s="1" t="s">
@@ -2773,7 +3207,7 @@
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="8"/>
+      <c r="A17" s="9"/>
       <c r="B17" s="1" t="s">
         <v>66</v>
       </c>
@@ -2788,7 +3222,7 @@
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="8"/>
+      <c r="A18" s="9"/>
       <c r="B18" s="1" t="s">
         <v>64</v>
       </c>
@@ -2814,12 +3248,888 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42A28763-695B-4824-893A-6B2282E51830}">
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="48.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>275</v>
+      </c>
+      <c r="B2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C2" t="s">
+        <v>276</v>
+      </c>
+      <c r="D2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>270</v>
+      </c>
+      <c r="B3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C3" t="s">
+        <v>271</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>273</v>
+      </c>
+      <c r="B4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C4" t="s">
+        <v>274</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>272</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77A8E0FF-7630-48F4-ADCF-8927F7DA3C25}">
+  <dimension ref="A1:E14"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="32.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="71.85546875" customWidth="1"/>
+    <col min="4" max="4" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="53.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>278</v>
+      </c>
+      <c r="B2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C2" t="s">
+        <v>286</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>280</v>
+      </c>
+      <c r="B3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C3" t="s">
+        <v>285</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>288</v>
+      </c>
+      <c r="B4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C4" t="s">
+        <v>290</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>281</v>
+      </c>
+      <c r="B5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C5" t="s">
+        <v>287</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>289</v>
+      </c>
+      <c r="B6" t="s">
+        <v>65</v>
+      </c>
+      <c r="C6" t="s">
+        <v>291</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>282</v>
+      </c>
+      <c r="B7" t="s">
+        <v>65</v>
+      </c>
+      <c r="C7" t="s">
+        <v>292</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>283</v>
+      </c>
+      <c r="B8" t="s">
+        <v>65</v>
+      </c>
+      <c r="C8" t="s">
+        <v>293</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>294</v>
+      </c>
+      <c r="B9" t="s">
+        <v>65</v>
+      </c>
+      <c r="C9" t="s">
+        <v>295</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>284</v>
+      </c>
+      <c r="B10" t="s">
+        <v>65</v>
+      </c>
+      <c r="C10" t="s">
+        <v>296</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>297</v>
+      </c>
+      <c r="B11" t="s">
+        <v>65</v>
+      </c>
+      <c r="C11" t="s">
+        <v>298</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>300</v>
+      </c>
+      <c r="B12" t="s">
+        <v>64</v>
+      </c>
+      <c r="C12" t="s">
+        <v>303</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>301</v>
+      </c>
+      <c r="B13" t="s">
+        <v>64</v>
+      </c>
+      <c r="C13" t="s">
+        <v>304</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>302</v>
+      </c>
+      <c r="B14" t="s">
+        <v>63</v>
+      </c>
+      <c r="C14" t="s">
+        <v>305</v>
+      </c>
+      <c r="D14">
+        <v>1.3</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E3DAA12-70CA-46C4-A60A-78495DA7491F}">
+  <dimension ref="A1:E23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="48.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
+        <v>359</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" t="s">
+        <v>397</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="9"/>
+      <c r="B3" s="10"/>
+      <c r="C3" t="s">
+        <v>398</v>
+      </c>
+      <c r="D3" s="10"/>
+      <c r="E3" s="9"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>326</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C4" t="s">
+        <v>367</v>
+      </c>
+      <c r="D4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E4" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>396</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>401</v>
+      </c>
+      <c r="C5" t="s">
+        <v>402</v>
+      </c>
+      <c r="D5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E5" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>394</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C6" t="s">
+        <v>404</v>
+      </c>
+      <c r="D6" t="s">
+        <v>30</v>
+      </c>
+      <c r="E6" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>395</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C7" t="s">
+        <v>406</v>
+      </c>
+      <c r="D7" t="s">
+        <v>407</v>
+      </c>
+      <c r="E7" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>325</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C8" t="s">
+        <v>368</v>
+      </c>
+      <c r="D8" t="s">
+        <v>30</v>
+      </c>
+      <c r="E8" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>341</v>
+      </c>
+      <c r="B9" t="s">
+        <v>65</v>
+      </c>
+      <c r="C9" t="s">
+        <v>126</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>342</v>
+      </c>
+      <c r="B10" t="s">
+        <v>65</v>
+      </c>
+      <c r="C10" t="s">
+        <v>127</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E10" s="9"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>343</v>
+      </c>
+      <c r="B11" t="s">
+        <v>65</v>
+      </c>
+      <c r="C11" t="s">
+        <v>128</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E11" s="9"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>344</v>
+      </c>
+      <c r="B12" t="s">
+        <v>65</v>
+      </c>
+      <c r="C12" t="s">
+        <v>129</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E12" s="9"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>345</v>
+      </c>
+      <c r="B13" t="s">
+        <v>65</v>
+      </c>
+      <c r="C13" t="s">
+        <v>130</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E13" s="9"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>346</v>
+      </c>
+      <c r="B14" t="s">
+        <v>65</v>
+      </c>
+      <c r="C14" t="s">
+        <v>131</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E14" s="9"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>347</v>
+      </c>
+      <c r="B15" t="s">
+        <v>65</v>
+      </c>
+      <c r="C15" t="s">
+        <v>132</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E15" s="9"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="9" t="s">
+        <v>371</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>411</v>
+      </c>
+      <c r="C16" t="s">
+        <v>412</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="E16" s="9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="9"/>
+      <c r="B17" s="9"/>
+      <c r="C17" t="s">
+        <v>413</v>
+      </c>
+      <c r="D17" s="10"/>
+      <c r="E17" s="9"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="9"/>
+      <c r="B18" s="9"/>
+      <c r="C18" s="3" t="s">
+        <v>414</v>
+      </c>
+      <c r="D18" s="10"/>
+      <c r="E18" s="9"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>372</v>
+      </c>
+      <c r="B19" t="s">
+        <v>411</v>
+      </c>
+      <c r="C19" t="s">
+        <v>415</v>
+      </c>
+      <c r="D19" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="E19" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>373</v>
+      </c>
+      <c r="B20" t="s">
+        <v>411</v>
+      </c>
+      <c r="C20" t="s">
+        <v>415</v>
+      </c>
+      <c r="D20" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="E20" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>374</v>
+      </c>
+      <c r="B21" t="s">
+        <v>411</v>
+      </c>
+      <c r="C21" t="s">
+        <v>415</v>
+      </c>
+      <c r="D21" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="E21" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>375</v>
+      </c>
+      <c r="B22" t="s">
+        <v>411</v>
+      </c>
+      <c r="C22" t="s">
+        <v>415</v>
+      </c>
+      <c r="D22" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="E22" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>366</v>
+      </c>
+      <c r="B23" t="s">
+        <v>369</v>
+      </c>
+      <c r="C23" t="s">
+        <v>370</v>
+      </c>
+      <c r="E23" t="s">
+        <v>416</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="9">
+    <mergeCell ref="E16:E18"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="E9:E15"/>
+    <mergeCell ref="A16:A18"/>
+    <mergeCell ref="B16:B18"/>
+    <mergeCell ref="D16:D18"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C14BA977-2416-4B6D-B8CC-F34F825401A3}">
+  <dimension ref="A1:D9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="58.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>323</v>
+      </c>
+      <c r="B2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C2" t="s">
+        <v>334</v>
+      </c>
+      <c r="D2" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>321</v>
+      </c>
+      <c r="B3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C3" t="s">
+        <v>331</v>
+      </c>
+      <c r="D3" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>318</v>
+      </c>
+      <c r="B4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C4" t="s">
+        <v>328</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>322</v>
+      </c>
+      <c r="B5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C5" t="s">
+        <v>333</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>320</v>
+      </c>
+      <c r="B6" t="s">
+        <v>65</v>
+      </c>
+      <c r="C6" t="s">
+        <v>330</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>319</v>
+      </c>
+      <c r="B7" t="s">
+        <v>65</v>
+      </c>
+      <c r="C7" t="s">
+        <v>329</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>324</v>
+      </c>
+      <c r="B8" t="s">
+        <v>64</v>
+      </c>
+      <c r="C8" t="s">
+        <v>335</v>
+      </c>
+      <c r="D8" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>317</v>
+      </c>
+      <c r="B9" t="s">
+        <v>65</v>
+      </c>
+      <c r="C9" t="s">
+        <v>327</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState ref="A2:D9">
+    <sortCondition ref="A2:A9"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DC55F79-79B3-4A74-88DE-7CAFD90BEB9A}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2843,7 +4153,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>279</v>
+        <v>338</v>
       </c>
       <c r="B2" t="s">
         <v>62</v>
@@ -2862,10 +4172,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1B8DBE5-887E-41ED-B9DC-6BC32D1444BD}">
-  <dimension ref="A1:E24"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2899,7 +4209,7 @@
         <v>27</v>
       </c>
       <c r="B2" t="s">
-        <v>139</v>
+        <v>125</v>
       </c>
       <c r="C2" t="s">
         <v>68</v>
@@ -2916,7 +4226,7 @@
         <v>28</v>
       </c>
       <c r="B3" t="s">
-        <v>139</v>
+        <v>125</v>
       </c>
       <c r="C3" t="s">
         <v>67</v>
@@ -2929,55 +4239,55 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="9" t="s">
         <v>64</v>
       </c>
       <c r="C4" t="s">
         <v>73</v>
       </c>
-      <c r="D4" s="9"/>
-      <c r="E4" s="8" t="s">
+      <c r="D4" s="10"/>
+      <c r="E4" s="9" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="8"/>
-      <c r="B5" s="8"/>
+      <c r="A5" s="9"/>
+      <c r="B5" s="9"/>
       <c r="C5" t="s">
         <v>70</v>
       </c>
-      <c r="D5" s="9"/>
-      <c r="E5" s="8"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="9"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="8"/>
-      <c r="B6" s="8"/>
+      <c r="A6" s="9"/>
+      <c r="B6" s="9"/>
       <c r="C6" t="s">
         <v>71</v>
       </c>
-      <c r="D6" s="9"/>
-      <c r="E6" s="8"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="9"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="8"/>
-      <c r="B7" s="8"/>
+      <c r="A7" s="9"/>
+      <c r="B7" s="9"/>
       <c r="C7" t="s">
         <v>72</v>
       </c>
-      <c r="D7" s="9"/>
-      <c r="E7" s="8"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="9"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="8"/>
-      <c r="B8" s="8"/>
+      <c r="A8" s="9"/>
+      <c r="B8" s="9"/>
       <c r="C8" t="s">
         <v>74</v>
       </c>
-      <c r="D8" s="9"/>
-      <c r="E8" s="8"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="9"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -2998,242 +4308,259 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>125</v>
+        <v>348</v>
       </c>
       <c r="B10" t="s">
         <v>65</v>
       </c>
       <c r="C10" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="E10" t="s">
-        <v>30</v>
-      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>126</v>
+        <v>349</v>
       </c>
       <c r="B11" t="s">
         <v>65</v>
       </c>
       <c r="C11" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="E11" t="s">
-        <v>30</v>
-      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>127</v>
+        <v>350</v>
       </c>
       <c r="B12" t="s">
         <v>65</v>
       </c>
       <c r="C12" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="E12" t="s">
-        <v>30</v>
-      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>128</v>
+        <v>351</v>
       </c>
       <c r="B13" t="s">
         <v>65</v>
       </c>
       <c r="C13" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="E13" t="s">
-        <v>30</v>
-      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>129</v>
+        <v>352</v>
       </c>
       <c r="B14" t="s">
         <v>65</v>
       </c>
       <c r="C14" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="E14" t="s">
-        <v>30</v>
-      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>130</v>
+        <v>353</v>
       </c>
       <c r="B15" t="s">
         <v>65</v>
       </c>
       <c r="C15" t="s">
-        <v>145</v>
+        <v>75</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>31</v>
       </c>
       <c r="E15" t="s">
-        <v>30</v>
+        <v>78</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>131</v>
-      </c>
-      <c r="B16" t="s">
+      <c r="A16" s="9" t="s">
+        <v>354</v>
+      </c>
+      <c r="B16" s="9" t="s">
         <v>65</v>
       </c>
       <c r="C16" t="s">
-        <v>146</v>
-      </c>
-      <c r="D16" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="D16" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="E16" t="s">
-        <v>30</v>
+      <c r="E16" s="9" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>134</v>
-      </c>
-      <c r="B17" t="s">
-        <v>65</v>
-      </c>
+      <c r="A17" s="9"/>
+      <c r="B17" s="9"/>
       <c r="C17" t="s">
-        <v>147</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>32</v>
-      </c>
+        <v>77</v>
+      </c>
+      <c r="D17" s="10"/>
+      <c r="E17" s="9"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>135</v>
+        <v>376</v>
       </c>
       <c r="B18" t="s">
-        <v>65</v>
+        <v>384</v>
       </c>
       <c r="C18" t="s">
-        <v>148</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>32</v>
+        <v>385</v>
+      </c>
+      <c r="D18" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="E18" s="13" t="s">
+        <v>392</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>136</v>
+        <v>377</v>
       </c>
       <c r="B19" t="s">
-        <v>65</v>
+        <v>384</v>
       </c>
       <c r="C19" t="s">
-        <v>149</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>32</v>
+        <v>385</v>
+      </c>
+      <c r="D19" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="E19" s="13" t="s">
+        <v>393</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>137</v>
+        <v>378</v>
       </c>
       <c r="B20" t="s">
-        <v>65</v>
+        <v>384</v>
       </c>
       <c r="C20" t="s">
-        <v>150</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>32</v>
+        <v>387</v>
+      </c>
+      <c r="D20" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="E20" s="13" t="s">
+        <v>392</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>138</v>
+        <v>379</v>
       </c>
       <c r="B21" t="s">
-        <v>65</v>
+        <v>384</v>
       </c>
       <c r="C21" t="s">
-        <v>151</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>32</v>
+        <v>389</v>
+      </c>
+      <c r="D21" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="E21" s="13" t="s">
+        <v>393</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>132</v>
+        <v>380</v>
       </c>
       <c r="B22" t="s">
-        <v>65</v>
+        <v>384</v>
       </c>
       <c r="C22" t="s">
-        <v>75</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="E22" t="s">
-        <v>78</v>
+        <v>386</v>
+      </c>
+      <c r="D22" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="E22" s="13" t="s">
+        <v>392</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="8" t="s">
-        <v>133</v>
-      </c>
-      <c r="B23" s="8" t="s">
-        <v>65</v>
+      <c r="A23" t="s">
+        <v>381</v>
+      </c>
+      <c r="B23" t="s">
+        <v>384</v>
       </c>
       <c r="C23" t="s">
-        <v>76</v>
-      </c>
-      <c r="D23" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="E23" s="8" t="s">
-        <v>79</v>
+        <v>388</v>
+      </c>
+      <c r="D23" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="E23" s="13" t="s">
+        <v>393</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="8"/>
-      <c r="B24" s="8"/>
+      <c r="A24" t="s">
+        <v>382</v>
+      </c>
+      <c r="B24" t="s">
+        <v>384</v>
+      </c>
       <c r="C24" t="s">
-        <v>77</v>
-      </c>
-      <c r="D24" s="9"/>
-      <c r="E24" s="8"/>
+        <v>391</v>
+      </c>
+      <c r="D24" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="E24" s="13" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>383</v>
+      </c>
+      <c r="B25" t="s">
+        <v>384</v>
+      </c>
+      <c r="C25" t="s">
+        <v>390</v>
+      </c>
+      <c r="D25" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="E25" s="13" t="s">
+        <v>393</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="D23:D24"/>
-    <mergeCell ref="E23:E24"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="E16:E17"/>
     <mergeCell ref="E4:E8"/>
     <mergeCell ref="A4:A8"/>
     <mergeCell ref="B4:B8"/>
@@ -3315,13 +4642,13 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>153</v>
+        <v>139</v>
       </c>
       <c r="B2" t="s">
-        <v>139</v>
+        <v>125</v>
       </c>
       <c r="C2" t="s">
-        <v>159</v>
+        <v>145</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>7</v>
@@ -3332,28 +4659,28 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>152</v>
+        <v>138</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>63</v>
       </c>
       <c r="C3" t="s">
-        <v>161</v>
+        <v>147</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="4" t="s">
-        <v>160</v>
+        <v>146</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>154</v>
+        <v>140</v>
       </c>
       <c r="B4" t="s">
         <v>63</v>
       </c>
       <c r="C4" t="s">
-        <v>162</v>
+        <v>148</v>
       </c>
       <c r="D4">
         <v>6.2</v>
@@ -3364,13 +4691,13 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>155</v>
+        <v>141</v>
       </c>
       <c r="B5" t="s">
         <v>63</v>
       </c>
       <c r="C5" t="s">
-        <v>163</v>
+        <v>149</v>
       </c>
       <c r="D5">
         <v>4.2</v>
@@ -3381,30 +4708,30 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>158</v>
+        <v>144</v>
       </c>
       <c r="B6" t="s">
         <v>62</v>
       </c>
       <c r="C6" t="s">
-        <v>141</v>
+        <v>127</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>32</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>160</v>
+        <v>146</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>156</v>
+        <v>142</v>
       </c>
       <c r="B7" t="s">
         <v>63</v>
       </c>
       <c r="C7" t="s">
-        <v>164</v>
+        <v>150</v>
       </c>
       <c r="D7">
         <v>2.2000000000000002</v>
@@ -3415,13 +4742,13 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>157</v>
+        <v>143</v>
       </c>
       <c r="B8" t="s">
         <v>63</v>
       </c>
       <c r="C8" t="s">
-        <v>165</v>
+        <v>151</v>
       </c>
       <c r="D8">
         <v>1.3</v>
@@ -3470,40 +4797,40 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
-        <v>166</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>167</v>
+      <c r="A2" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>153</v>
       </c>
       <c r="C2" t="s">
-        <v>168</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>170</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>171</v>
+        <v>154</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>156</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="8"/>
-      <c r="B3" s="8"/>
+      <c r="A3" s="9"/>
+      <c r="B3" s="9"/>
       <c r="C3" t="s">
-        <v>169</v>
-      </c>
-      <c r="D3" s="9"/>
-      <c r="E3" s="8"/>
+        <v>155</v>
+      </c>
+      <c r="D3" s="10"/>
+      <c r="E3" s="9"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>172</v>
+        <v>158</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>65</v>
       </c>
       <c r="C4" t="s">
-        <v>173</v>
+        <v>159</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>31</v>
@@ -3514,16 +4841,16 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>174</v>
+        <v>160</v>
       </c>
       <c r="B5" t="s">
-        <v>185</v>
+        <v>171</v>
       </c>
       <c r="C5" t="s">
-        <v>179</v>
+        <v>165</v>
       </c>
       <c r="D5" t="s">
-        <v>180</v>
+        <v>166</v>
       </c>
       <c r="E5" t="s">
         <v>30</v>
@@ -3531,13 +4858,13 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>175</v>
+        <v>161</v>
       </c>
       <c r="B6" t="s">
         <v>63</v>
       </c>
       <c r="C6" t="s">
-        <v>181</v>
+        <v>167</v>
       </c>
       <c r="D6">
         <v>1.5</v>
@@ -3548,13 +4875,13 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>176</v>
+        <v>162</v>
       </c>
       <c r="B7" t="s">
-        <v>185</v>
+        <v>171</v>
       </c>
       <c r="C7" t="s">
-        <v>182</v>
+        <v>168</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>32</v>
@@ -3565,16 +4892,16 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>177</v>
+        <v>163</v>
       </c>
       <c r="B8" t="s">
         <v>65</v>
       </c>
       <c r="C8" t="s">
-        <v>183</v>
+        <v>169</v>
       </c>
       <c r="D8" t="s">
-        <v>184</v>
+        <v>170</v>
       </c>
       <c r="E8" t="s">
         <v>30</v>
@@ -3582,19 +4909,19 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>178</v>
+        <v>164</v>
       </c>
       <c r="B9" t="s">
         <v>63</v>
       </c>
       <c r="C9" t="s">
-        <v>186</v>
+        <v>172</v>
       </c>
       <c r="D9">
         <v>7</v>
       </c>
       <c r="E9" t="s">
-        <v>187</v>
+        <v>173</v>
       </c>
     </row>
   </sheetData>
@@ -3644,30 +4971,30 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>200</v>
+        <v>339</v>
       </c>
       <c r="B2" t="s">
-        <v>201</v>
+        <v>186</v>
       </c>
       <c r="C2" t="s">
-        <v>202</v>
+        <v>187</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>203</v>
+        <v>188</v>
       </c>
       <c r="E2" t="s">
-        <v>204</v>
+        <v>189</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>205</v>
+        <v>340</v>
       </c>
       <c r="B3" t="s">
         <v>65</v>
       </c>
       <c r="C3" t="s">
-        <v>206</v>
+        <v>190</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>32</v>
@@ -3683,10 +5010,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCA3E29C-4580-4CDD-8302-895C0D68B708}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3723,24 +5050,24 @@
         <v>62</v>
       </c>
       <c r="C2" t="s">
-        <v>188</v>
+        <v>174</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>30</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>189</v>
+        <v>175</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>192</v>
+        <v>178</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>185</v>
+        <v>171</v>
       </c>
       <c r="C3" t="s">
-        <v>190</v>
+        <v>176</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>13</v>
@@ -3751,13 +5078,13 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>193</v>
+        <v>179</v>
       </c>
       <c r="B4" t="s">
         <v>65</v>
       </c>
       <c r="C4" t="s">
-        <v>191</v>
+        <v>177</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>31</v>
@@ -3768,13 +5095,13 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>194</v>
+        <v>180</v>
       </c>
       <c r="B5" t="s">
         <v>63</v>
       </c>
       <c r="C5" t="s">
-        <v>198</v>
+        <v>184</v>
       </c>
       <c r="D5">
         <v>12</v>
@@ -3785,13 +5112,13 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>195</v>
+        <v>181</v>
       </c>
       <c r="B6" t="s">
         <v>62</v>
       </c>
       <c r="C6" t="s">
-        <v>199</v>
+        <v>185</v>
       </c>
       <c r="D6" s="3">
         <v>10</v>
@@ -3802,18 +5129,49 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>196</v>
+        <v>360</v>
       </c>
       <c r="B7" t="s">
+        <v>362</v>
+      </c>
+      <c r="C7" t="s">
+        <v>363</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E7" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
+        <v>361</v>
+      </c>
+      <c r="B8" t="s">
+        <v>362</v>
+      </c>
+      <c r="C8" t="s">
+        <v>364</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
+        <v>182</v>
+      </c>
+      <c r="B9" t="s">
         <v>65</v>
       </c>
-      <c r="C7" t="s">
-        <v>197</v>
-      </c>
-      <c r="D7" s="3" t="s">
+      <c r="C9" t="s">
+        <v>183</v>
+      </c>
+      <c r="D9" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E9" t="s">
         <v>30</v>
       </c>
     </row>

</xml_diff>

<commit_message>
doc update for contour + gantt
</commit_message>
<xml_diff>
--- a/fivecentplots/keywords.xlsx
+++ b/fivecentplots/keywords.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="13"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="19"/>
   </bookViews>
   <sheets>
     <sheet name="Mandatory" sheetId="1" state="visible" r:id="rId2"/>
@@ -26,14 +26,15 @@
     <sheet name="BoxDiamond" sheetId="16" state="visible" r:id="rId17"/>
     <sheet name="BoxViolin" sheetId="17" state="visible" r:id="rId18"/>
     <sheet name="Bar" sheetId="18" state="visible" r:id="rId19"/>
-    <sheet name="WS" sheetId="19" state="visible" r:id="rId20"/>
-    <sheet name="Cbar" sheetId="20" state="visible" r:id="rId21"/>
-    <sheet name="Contour" sheetId="21" state="visible" r:id="rId22"/>
-    <sheet name="Heatmap" sheetId="22" state="visible" r:id="rId23"/>
-    <sheet name="Stats" sheetId="23" state="visible" r:id="rId24"/>
-    <sheet name="Gridlines" sheetId="24" state="visible" r:id="rId25"/>
-    <sheet name="Data" sheetId="25" state="visible" r:id="rId26"/>
-    <sheet name="Other" sheetId="26" state="visible" r:id="rId27"/>
+    <sheet name="Contour" sheetId="19" state="visible" r:id="rId20"/>
+    <sheet name="Gantt" sheetId="20" state="visible" r:id="rId21"/>
+    <sheet name="WS" sheetId="21" state="visible" r:id="rId22"/>
+    <sheet name="Cbar" sheetId="22" state="visible" r:id="rId23"/>
+    <sheet name="Heatmap" sheetId="23" state="visible" r:id="rId24"/>
+    <sheet name="Stats" sheetId="24" state="visible" r:id="rId25"/>
+    <sheet name="Gridlines" sheetId="25" state="visible" r:id="rId26"/>
+    <sheet name="Data" sheetId="26" state="visible" r:id="rId27"/>
+    <sheet name="Other" sheetId="27" state="visible" r:id="rId28"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -45,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2216" uniqueCount="615">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2285" uniqueCount="651">
   <si>
     <t xml:space="preserve">Keyword</t>
   </si>
@@ -1409,6 +1410,191 @@
     <t xml:space="preserve">Width for the rolling mean line in pixels</t>
   </si>
   <si>
+    <t xml:space="preserve">contour_width</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Width of the contour lines</t>
+  </si>
+  <si>
+    <t xml:space="preserve">contour.html#Contour-lines</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cmap</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Name of a color map </t>
+  </si>
+  <si>
+    <t xml:space="preserve">inferno</t>
+  </si>
+  <si>
+    <t xml:space="preserve">contour.html#Filled-contour</t>
+  </si>
+  <si>
+    <t xml:space="preserve">filled</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Color area between contour lines</t>
+  </si>
+  <si>
+    <t xml:space="preserve">levels</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number of contour lines/levels to draw</t>
+  </si>
+  <si>
+    <t xml:space="preserve">interp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Scipy interpolate.griddata method to make Z points {‘linear’, ‘nearest’, ‘cubic’}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">'cubic’</t>
+  </si>
+  <si>
+    <t xml:space="preserve">contour.html#Data-interpolation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">show_points</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Show points on top of the contour plot</t>
+  </si>
+  <si>
+    <t xml:space="preserve">contour.html#Contour-points</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gantt_color_by_bar | color_by_bar</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Color each </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Gantt</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> bar differently</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">gantt.html#Styling</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gantt_height | height</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Set the fractional height of the Gantt bars between 0-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gantt_edge_color</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hex color string for the edge of the Gantt bars</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gantt_edge_width</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Width of the edge of the </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Gantt</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> bars in pixels</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">gantt_order_by_legend | order by legend</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Order the y-axis values based on the sort order of the legend values [requires legend]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gantt.html#Legends</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gantt_fill_alpha</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transparency value for the Gantt bars between 0-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gantt_fill_color</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hex color string of the Gantt bar fill </t>
+  </si>
+  <si>
+    <t xml:space="preserve">gantt_label_x</t>
+  </si>
+  <si>
+    <t xml:space="preserve">By default, x-axis labels are disabled for this plot type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">'’</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gantt_tick_labels_x_rotation | tick_labels_x_rotation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gantt-specific version of the this kwarg to ensure rotations are not applied globably to all plots from a theme file</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sort</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sort order for the Gantt bars {‘ascending’, ‘descending’}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">'descending’</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gantt.html#Sorting</t>
+  </si>
+  <si>
     <t xml:space="preserve">Row/column grid</t>
   </si>
   <si>
@@ -1517,43 +1703,22 @@
     <t xml:space="preserve">cbar</t>
   </si>
   <si>
+    <t xml:space="preserve">Toggle colorbar on/off for contour and heatmap plots</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cbar width [height will match the height of the axes]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cell_size</t>
+  </si>
+  <si>
+    <t xml:space="preserve">width of a heatmap cell</t>
+  </si>
+  <si>
+    <t xml:space="preserve">`cell size &lt;heatmap.html#Cell-size&gt;`_</t>
+  </si>
+  <si>
     <t xml:space="preserve">toggle colorbar on/off for contour and heatmap plots</t>
-  </si>
-  <si>
-    <t xml:space="preserve">`contour example &lt;contour.html#Filled-contour&gt;`_</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cbar width (height will match the height of the axes)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cmap</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Name of a color map </t>
-  </si>
-  <si>
-    <t xml:space="preserve">inferno</t>
-  </si>
-  <si>
-    <t xml:space="preserve">filled</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fill area between contour lines</t>
-  </si>
-  <si>
-    <t xml:space="preserve">levels</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Number of contour lines/levels to draw</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cell_size</t>
-  </si>
-  <si>
-    <t xml:space="preserve">width of a heatmap cell</t>
-  </si>
-  <si>
-    <t xml:space="preserve">`cell size &lt;heatmap.html#Cell-size&gt;`_</t>
   </si>
   <si>
     <t xml:space="preserve">`basic heatmap &lt;heatmap.html#No-data-labels&gt;`_</t>
@@ -1900,7 +2065,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1922,6 +2087,12 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -2022,7 +2193,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2034,7 +2205,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3294,7 +3465,7 @@
   </sheetPr>
   <dimension ref="A1:AMJ11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
     </sheetView>
   </sheetViews>
@@ -7325,8 +7496,8 @@
   </sheetPr>
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E10" activeCellId="0" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7411,7 +7582,7 @@
         <v>427</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>71</v>
+        <v>21</v>
       </c>
       <c r="C5" s="0" t="s">
         <v>428</v>
@@ -7433,9 +7604,8 @@
       <c r="C6" s="0" t="s">
         <v>430</v>
       </c>
-      <c r="D6" s="12" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+      <c r="D6" s="12" t="s">
+        <v>104</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>431</v>
@@ -7610,250 +7780,139 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
+      <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="56.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="33.47"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="44.49"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="B1" s="5" t="s">
         <v>0</v>
       </c>
+      <c r="B1" s="0" t="s">
+        <v>1</v>
+      </c>
       <c r="C1" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>454</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>455</v>
+      </c>
+      <c r="D2" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="D1" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="0" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
-        <v>454</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>455</v>
-      </c>
-      <c r="C2" s="1" t="s">
+      <c r="E2" s="0" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>457</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>458</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>459</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>461</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>228</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>462</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>463</v>
+      </c>
+      <c r="B5" s="0" t="s">
         <v>71</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="C5" s="0" t="s">
+        <v>464</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="E5" s="0" t="s">
         <v>456</v>
       </c>
-      <c r="E2" s="0" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1"/>
-      <c r="B3" s="0" t="s">
-        <v>457</v>
-      </c>
-      <c r="C3" s="1"/>
-      <c r="D3" s="0" t="s">
-        <v>458</v>
-      </c>
-      <c r="E3" s="0" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1"/>
-      <c r="B4" s="0" t="s">
-        <v>459</v>
-      </c>
-      <c r="C4" s="1"/>
-      <c r="D4" s="0" t="s">
-        <v>460</v>
-      </c>
-      <c r="E4" s="0" t="n">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1"/>
-      <c r="B5" s="0" t="s">
-        <v>461</v>
-      </c>
-      <c r="C5" s="1"/>
-      <c r="D5" s="0" t="s">
-        <v>462</v>
-      </c>
-      <c r="E5" s="0" t="n">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
-        <v>463</v>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>465</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>464</v>
-      </c>
-      <c r="C6" s="1"/>
+        <v>9</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>466</v>
+      </c>
       <c r="D6" s="0" t="s">
-        <v>465</v>
-      </c>
-      <c r="E6" s="0" t="n">
-        <v>10</v>
+        <v>467</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>468</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1"/>
+      <c r="A7" s="0" t="s">
+        <v>469</v>
+      </c>
       <c r="B7" s="0" t="s">
-        <v>466</v>
-      </c>
-      <c r="C7" s="1"/>
+        <v>228</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>470</v>
+      </c>
       <c r="D7" s="0" t="s">
-        <v>467</v>
-      </c>
-      <c r="E7" s="0" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1"/>
-      <c r="B8" s="0" t="s">
-        <v>468</v>
-      </c>
-      <c r="C8" s="1"/>
-      <c r="D8" s="0" t="s">
-        <v>469</v>
-      </c>
-      <c r="E8" s="0" t="n">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1"/>
-      <c r="B9" s="0" t="s">
-        <v>470</v>
-      </c>
-      <c r="C9" s="1"/>
-      <c r="D9" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="E7" s="0" t="s">
         <v>471</v>
       </c>
-      <c r="E9" s="0" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="s">
-        <v>472</v>
-      </c>
-      <c r="B10" s="0" t="s">
-        <v>473</v>
-      </c>
-      <c r="C10" s="1"/>
-      <c r="D10" s="0" t="s">
-        <v>474</v>
-      </c>
-      <c r="E10" s="0" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1"/>
-      <c r="B11" s="0" t="s">
-        <v>475</v>
-      </c>
-      <c r="C11" s="1"/>
-      <c r="D11" s="0" t="s">
-        <v>476</v>
-      </c>
-      <c r="E11" s="0" t="n">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1"/>
-      <c r="B12" s="0" t="s">
-        <v>477</v>
-      </c>
-      <c r="C12" s="1"/>
-      <c r="D12" s="0" t="s">
-        <v>478</v>
-      </c>
-      <c r="E12" s="0" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1"/>
-      <c r="B13" s="0" t="s">
-        <v>479</v>
-      </c>
-      <c r="C13" s="1"/>
-      <c r="D13" s="0" t="s">
-        <v>480</v>
-      </c>
-      <c r="E13" s="0" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1"/>
-      <c r="B14" s="0" t="s">
-        <v>481</v>
-      </c>
-      <c r="C14" s="1"/>
-      <c r="D14" s="0" t="s">
-        <v>482</v>
-      </c>
-      <c r="E14" s="0" t="n">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
-        <v>483</v>
-      </c>
-      <c r="B15" s="0" t="s">
-        <v>484</v>
-      </c>
-      <c r="C15" s="1"/>
-      <c r="D15" s="0" t="s">
-        <v>485</v>
-      </c>
-      <c r="E15" s="0" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
-        <v>486</v>
-      </c>
-      <c r="B16" s="0" t="s">
-        <v>487</v>
-      </c>
-      <c r="C16" s="1"/>
-      <c r="D16" s="0" t="s">
-        <v>488</v>
-      </c>
-      <c r="E16" s="0" t="n">
-        <v>10</v>
-      </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="A2:A5"/>
-    <mergeCell ref="C2:C16"/>
-    <mergeCell ref="A6:A9"/>
-    <mergeCell ref="A10:A14"/>
-  </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -8186,18 +8245,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E12" activeCellId="0" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="48.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="48.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="11" width="19.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="5" width="40.14"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
@@ -8207,45 +8270,188 @@
       <c r="C1" s="0" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="5" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
+        <v>472</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>228</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>473</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>475</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>476</v>
+      </c>
+      <c r="D3" s="11" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>477</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>478</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>409</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>479</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>480</v>
+      </c>
+      <c r="D5" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>481</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>228</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>482</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>484</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>485</v>
+      </c>
+      <c r="D7" s="11" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>486</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>487</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>409</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>488</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="0" t="s">
         <v>489</v>
       </c>
-      <c r="B2" s="0" t="s">
-        <v>59</v>
-      </c>
-      <c r="C2" s="0" t="s">
+      <c r="D9" s="12" t="s">
         <v>490</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="E2" s="14" t="s">
+      <c r="E9" s="5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
         <v>491</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>64</v>
-      </c>
-      <c r="B3" s="0" t="s">
+      <c r="B10" s="0" t="s">
         <v>71</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C10" s="0" t="s">
         <v>492</v>
       </c>
-      <c r="D3" s="3" t="n">
-        <v>30</v>
-      </c>
-      <c r="E3" s="14"/>
-    </row>
+      <c r="D10" s="11" t="n">
+        <v>90</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>493</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>494</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>495</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -8262,13 +8468,275 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="56.42"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>497</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>498</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>499</v>
+      </c>
+      <c r="E2" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1"/>
+      <c r="B3" s="0" t="s">
+        <v>500</v>
+      </c>
+      <c r="C3" s="1"/>
+      <c r="D3" s="0" t="s">
+        <v>501</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1"/>
+      <c r="B4" s="0" t="s">
+        <v>502</v>
+      </c>
+      <c r="C4" s="1"/>
+      <c r="D4" s="0" t="s">
+        <v>503</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1"/>
+      <c r="B5" s="0" t="s">
+        <v>504</v>
+      </c>
+      <c r="C5" s="1"/>
+      <c r="D5" s="0" t="s">
+        <v>505</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>506</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>507</v>
+      </c>
+      <c r="C6" s="1"/>
+      <c r="D6" s="0" t="s">
+        <v>508</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1"/>
+      <c r="B7" s="0" t="s">
+        <v>509</v>
+      </c>
+      <c r="C7" s="1"/>
+      <c r="D7" s="0" t="s">
+        <v>510</v>
+      </c>
+      <c r="E7" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1"/>
+      <c r="B8" s="0" t="s">
+        <v>511</v>
+      </c>
+      <c r="C8" s="1"/>
+      <c r="D8" s="0" t="s">
+        <v>512</v>
+      </c>
+      <c r="E8" s="0" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1"/>
+      <c r="B9" s="0" t="s">
+        <v>513</v>
+      </c>
+      <c r="C9" s="1"/>
+      <c r="D9" s="0" t="s">
+        <v>514</v>
+      </c>
+      <c r="E9" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>515</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>516</v>
+      </c>
+      <c r="C10" s="1"/>
+      <c r="D10" s="0" t="s">
+        <v>517</v>
+      </c>
+      <c r="E10" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1"/>
+      <c r="B11" s="0" t="s">
+        <v>518</v>
+      </c>
+      <c r="C11" s="1"/>
+      <c r="D11" s="0" t="s">
+        <v>519</v>
+      </c>
+      <c r="E11" s="0" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1"/>
+      <c r="B12" s="0" t="s">
+        <v>520</v>
+      </c>
+      <c r="C12" s="1"/>
+      <c r="D12" s="0" t="s">
+        <v>521</v>
+      </c>
+      <c r="E12" s="0" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1"/>
+      <c r="B13" s="0" t="s">
+        <v>522</v>
+      </c>
+      <c r="C13" s="1"/>
+      <c r="D13" s="0" t="s">
+        <v>523</v>
+      </c>
+      <c r="E13" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1"/>
+      <c r="B14" s="0" t="s">
+        <v>524</v>
+      </c>
+      <c r="C14" s="1"/>
+      <c r="D14" s="0" t="s">
+        <v>525</v>
+      </c>
+      <c r="E14" s="0" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>526</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>527</v>
+      </c>
+      <c r="C15" s="1"/>
+      <c r="D15" s="0" t="s">
+        <v>528</v>
+      </c>
+      <c r="E15" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>529</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>530</v>
+      </c>
+      <c r="C16" s="1"/>
+      <c r="D16" s="0" t="s">
+        <v>531</v>
+      </c>
+      <c r="E16" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="C2:C16"/>
+    <mergeCell ref="A6:A9"/>
+    <mergeCell ref="A10:A14"/>
+  </mergeCells>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:E1048576"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="48.85"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -8289,50 +8757,39 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>493</v>
+        <v>532</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>9</v>
+        <v>228</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>494</v>
+        <v>533</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>495</v>
+        <v>104</v>
       </c>
       <c r="E2" s="14" t="s">
-        <v>491</v>
+        <v>460</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>496</v>
+        <v>64</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>59</v>
+        <v>71</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>497</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="E3" s="14"/>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>498</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="C4" s="0" t="s">
-        <v>499</v>
-      </c>
-      <c r="D4" s="0" t="n">
-        <v>20</v>
-      </c>
-    </row>
+        <v>534</v>
+      </c>
+      <c r="D3" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -8344,7 +8801,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -8383,67 +8840,67 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="15" t="s">
-        <v>500</v>
+        <v>535</v>
       </c>
       <c r="B2" s="0" t="s">
         <v>71</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>501</v>
+        <v>536</v>
       </c>
       <c r="D2" s="3" t="n">
         <v>60</v>
       </c>
       <c r="E2" s="14" t="s">
-        <v>502</v>
+        <v>537</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>493</v>
+        <v>457</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>59</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>490</v>
+        <v>538</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>104</v>
       </c>
       <c r="E3" s="14" t="s">
-        <v>503</v>
+        <v>539</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>504</v>
+        <v>540</v>
       </c>
       <c r="B4" s="0" t="s">
         <v>59</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>505</v>
+        <v>541</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>104</v>
       </c>
       <c r="E4" s="14" t="s">
-        <v>506</v>
+        <v>542</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>507</v>
+        <v>543</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>508</v>
+        <v>544</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>509</v>
+        <v>545</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>510</v>
+        <v>546</v>
       </c>
       <c r="E5" s="14" t="s">
         <v>69</v>
@@ -8460,7 +8917,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -8495,53 +8952,53 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>511</v>
+        <v>547</v>
       </c>
       <c r="B2" s="0" t="s">
         <v>21</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>512</v>
+        <v>548</v>
       </c>
       <c r="D2" s="0" t="s">
         <v>69</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>513</v>
+        <v>549</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>514</v>
+        <v>550</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>9</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>515</v>
+        <v>551</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>69</v>
       </c>
       <c r="E3" s="14" t="s">
-        <v>516</v>
+        <v>552</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>517</v>
+        <v>553</v>
       </c>
       <c r="B4" s="0" t="s">
         <v>9</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>518</v>
+        <v>554</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>69</v>
       </c>
       <c r="E4" s="14" t="s">
-        <v>516</v>
+        <v>552</v>
       </c>
     </row>
   </sheetData>
@@ -8555,7 +9012,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -8594,30 +9051,30 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>519</v>
+        <v>555</v>
       </c>
       <c r="B2" s="0" t="s">
         <v>59</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>520</v>
+        <v>556</v>
       </c>
       <c r="D2" s="14" t="s">
         <v>93</v>
       </c>
       <c r="E2" s="14" t="s">
-        <v>521</v>
+        <v>557</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>522</v>
+        <v>558</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>59</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>523</v>
+        <v>559</v>
       </c>
       <c r="D3" s="14" t="s">
         <v>93</v>
@@ -8628,13 +9085,13 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>524</v>
+        <v>560</v>
       </c>
       <c r="B4" s="0" t="s">
         <v>59</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>525</v>
+        <v>561</v>
       </c>
       <c r="D4" s="14" t="s">
         <v>104</v>
@@ -8645,13 +9102,13 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>526</v>
+        <v>562</v>
       </c>
       <c r="B5" s="0" t="s">
         <v>59</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>527</v>
+        <v>563</v>
       </c>
       <c r="D5" s="14" t="s">
         <v>93</v>
@@ -8662,13 +9119,13 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>528</v>
+        <v>564</v>
       </c>
       <c r="B6" s="0" t="s">
         <v>59</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>529</v>
+        <v>565</v>
       </c>
       <c r="D6" s="14" t="s">
         <v>104</v>
@@ -8679,30 +9136,30 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>530</v>
+        <v>566</v>
       </c>
       <c r="B7" s="0" t="s">
         <v>59</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>531</v>
+        <v>567</v>
       </c>
       <c r="D7" s="14" t="s">
         <v>104</v>
       </c>
       <c r="E7" s="14" t="s">
-        <v>532</v>
+        <v>568</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>533</v>
+        <v>569</v>
       </c>
       <c r="B8" s="0" t="s">
         <v>59</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>534</v>
+        <v>570</v>
       </c>
       <c r="D8" s="14" t="s">
         <v>104</v>
@@ -8713,13 +9170,13 @@
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>535</v>
+        <v>571</v>
       </c>
       <c r="B9" s="0" t="s">
         <v>59</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>536</v>
+        <v>572</v>
       </c>
       <c r="D9" s="14" t="s">
         <v>104</v>
@@ -8730,13 +9187,13 @@
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>537</v>
+        <v>573</v>
       </c>
       <c r="B10" s="0" t="s">
         <v>59</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>538</v>
+        <v>574</v>
       </c>
       <c r="D10" s="14" t="s">
         <v>104</v>
@@ -8747,13 +9204,13 @@
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>539</v>
+        <v>575</v>
       </c>
       <c r="B11" s="0" t="s">
         <v>59</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>540</v>
+        <v>576</v>
       </c>
       <c r="D11" s="14" t="s">
         <v>104</v>
@@ -8764,13 +9221,13 @@
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>541</v>
+        <v>577</v>
       </c>
       <c r="B12" s="0" t="s">
         <v>9</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>542</v>
+        <v>578</v>
       </c>
       <c r="D12" s="14" t="s">
         <v>26</v>
@@ -8781,13 +9238,13 @@
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>543</v>
+        <v>579</v>
       </c>
       <c r="B13" s="0" t="s">
         <v>9</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>544</v>
+        <v>580</v>
       </c>
       <c r="D13" s="14" t="s">
         <v>55</v>
@@ -8798,13 +9255,13 @@
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>545</v>
+        <v>581</v>
       </c>
       <c r="B14" s="0" t="s">
         <v>21</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>546</v>
+        <v>582</v>
       </c>
       <c r="D14" s="0" t="n">
         <v>1.3</v>
@@ -8824,7 +9281,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -8860,135 +9317,135 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>547</v>
+        <v>583</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>93</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>548</v>
+        <v>584</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>93</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>549</v>
+        <v>585</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="0" t="s">
-        <v>550</v>
+        <v>586</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>551</v>
+        <v>587</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>552</v>
+        <v>588</v>
       </c>
       <c r="D4" s="0" t="s">
         <v>69</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>553</v>
+        <v>589</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>554</v>
+        <v>590</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>555</v>
+        <v>591</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>556</v>
+        <v>592</v>
       </c>
       <c r="D5" s="0" t="s">
         <v>69</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>557</v>
+        <v>593</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>558</v>
+        <v>594</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>559</v>
+        <v>595</v>
       </c>
       <c r="D6" s="0" t="s">
         <v>69</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>560</v>
+        <v>596</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>561</v>
+        <v>597</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>71</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>562</v>
+        <v>598</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>563</v>
+        <v>599</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>564</v>
+        <v>600</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>565</v>
+        <v>601</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>566</v>
+        <v>602</v>
       </c>
       <c r="D8" s="0" t="s">
         <v>69</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>567</v>
+        <v>603</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>568</v>
+        <v>604</v>
       </c>
       <c r="B9" s="0" t="s">
         <v>59</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>569</v>
+        <v>605</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>93</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>570</v>
+        <v>606</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>571</v>
+        <v>607</v>
       </c>
       <c r="B10" s="0" t="s">
         <v>59</v>
@@ -9003,13 +9460,13 @@
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>572</v>
+        <v>608</v>
       </c>
       <c r="B11" s="0" t="s">
         <v>59</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>573</v>
+        <v>609</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>93</v>
@@ -9018,13 +9475,13 @@
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>574</v>
+        <v>610</v>
       </c>
       <c r="B12" s="0" t="s">
         <v>59</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>575</v>
+        <v>611</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>93</v>
@@ -9033,13 +9490,13 @@
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>576</v>
+        <v>612</v>
       </c>
       <c r="B13" s="0" t="s">
         <v>59</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>577</v>
+        <v>613</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>93</v>
@@ -9048,13 +9505,13 @@
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>578</v>
+        <v>614</v>
       </c>
       <c r="B14" s="0" t="s">
         <v>59</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>579</v>
+        <v>615</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>104</v>
@@ -9063,13 +9520,13 @@
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>580</v>
+        <v>616</v>
       </c>
       <c r="B15" s="0" t="s">
         <v>59</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>581</v>
+        <v>617</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>104</v>
@@ -9078,13 +9535,13 @@
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>582</v>
+        <v>618</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>583</v>
+        <v>619</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>584</v>
+        <v>620</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>69</v>
@@ -9097,7 +9554,7 @@
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="0" t="s">
-        <v>585</v>
+        <v>621</v>
       </c>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
@@ -9106,20 +9563,20 @@
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="3" t="s">
-        <v>586</v>
+        <v>622</v>
       </c>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>587</v>
+        <v>623</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>583</v>
+        <v>619</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>588</v>
+        <v>624</v>
       </c>
       <c r="D19" s="4" t="s">
         <v>69</v>
@@ -9130,13 +9587,13 @@
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>589</v>
+        <v>625</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>583</v>
+        <v>619</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>588</v>
+        <v>624</v>
       </c>
       <c r="D20" s="4" t="s">
         <v>69</v>
@@ -9147,13 +9604,13 @@
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>590</v>
+        <v>626</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>583</v>
+        <v>619</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>588</v>
+        <v>624</v>
       </c>
       <c r="D21" s="4" t="s">
         <v>69</v>
@@ -9164,13 +9621,13 @@
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>591</v>
+        <v>627</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>583</v>
+        <v>619</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>588</v>
+        <v>624</v>
       </c>
       <c r="D22" s="4" t="s">
         <v>69</v>
@@ -9181,16 +9638,16 @@
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>592</v>
+        <v>628</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>593</v>
+        <v>629</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>594</v>
+        <v>630</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>595</v>
+        <v>631</v>
       </c>
     </row>
   </sheetData>
@@ -9215,7 +9672,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -9248,41 +9705,41 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>596</v>
+        <v>632</v>
       </c>
       <c r="B2" s="0" t="s">
         <v>9</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>597</v>
+        <v>633</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>598</v>
+        <v>634</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>599</v>
+        <v>635</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>9</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>600</v>
+        <v>636</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>601</v>
+        <v>637</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>602</v>
+        <v>638</v>
       </c>
       <c r="B4" s="0" t="s">
         <v>59</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>603</v>
+        <v>639</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>93</v>
@@ -9290,13 +9747,13 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>604</v>
+        <v>640</v>
       </c>
       <c r="B5" s="0" t="s">
         <v>59</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>605</v>
+        <v>641</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>104</v>
@@ -9304,13 +9761,13 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>606</v>
+        <v>642</v>
       </c>
       <c r="B6" s="0" t="s">
         <v>59</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>607</v>
+        <v>643</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>104</v>
@@ -9318,13 +9775,13 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>608</v>
+        <v>644</v>
       </c>
       <c r="B7" s="0" t="s">
         <v>59</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>609</v>
+        <v>645</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>93</v>
@@ -9332,27 +9789,27 @@
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>610</v>
+        <v>646</v>
       </c>
       <c r="B8" s="0" t="s">
         <v>9</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>611</v>
+        <v>647</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>612</v>
+        <v>648</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>613</v>
+        <v>649</v>
       </c>
       <c r="B9" s="0" t="s">
         <v>59</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>614</v>
+        <v>650</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>104</v>

</xml_diff>

<commit_message>
heatmap docs and update
</commit_message>
<xml_diff>
--- a/fivecentplots/keywords.xlsx
+++ b/fivecentplots/keywords.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="19"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="22"/>
   </bookViews>
   <sheets>
     <sheet name="Mandatory" sheetId="1" state="visible" r:id="rId2"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2285" uniqueCount="651">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2298" uniqueCount="656">
   <si>
     <t xml:space="preserve">Keyword</t>
   </si>
@@ -1467,35 +1467,7 @@
     <t xml:space="preserve">gantt_color_by_bar | color_by_bar</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Color each </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Gantt</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> bar differently</t>
-    </r>
+    <t xml:space="preserve">Color each Gantt bar differently</t>
   </si>
   <si>
     <t xml:space="preserve">gantt.html#Styling</t>
@@ -1516,35 +1488,7 @@
     <t xml:space="preserve">gantt_edge_width</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Width of the edge of the </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Gantt</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> bars in pixels</t>
-    </r>
+    <t xml:space="preserve">Width of the edge of the Gantt bars in pixels</t>
   </si>
   <si>
     <t xml:space="preserve">gantt_order_by_legend | order by legend</t>
@@ -1712,13 +1656,13 @@
     <t xml:space="preserve">cell_size</t>
   </si>
   <si>
-    <t xml:space="preserve">width of a heatmap cell</t>
+    <t xml:space="preserve">Width of a heatmap cell in pixels</t>
   </si>
   <si>
     <t xml:space="preserve">`cell size &lt;heatmap.html#Cell-size&gt;`_</t>
   </si>
   <si>
-    <t xml:space="preserve">toggle colorbar on/off for contour and heatmap plots</t>
+    <t xml:space="preserve">Name of a color map to apply to the plot</t>
   </si>
   <si>
     <t xml:space="preserve">`basic heatmap &lt;heatmap.html#No-data-labels&gt;`_</t>
@@ -1727,22 +1671,37 @@
     <t xml:space="preserve">data_labels</t>
   </si>
   <si>
-    <t xml:space="preserve">enable/disable value labels on the heatmap cells</t>
+    <t xml:space="preserve">Toggle visibility of value text labels on the heatmap cells</t>
   </si>
   <si>
     <t xml:space="preserve">`data labels &lt;heatmap.html#With-data-labels&gt;`_</t>
   </si>
   <si>
-    <t xml:space="preserve">heatmap_font_xxx</t>
-  </si>
-  <si>
-    <t xml:space="preserve">various</t>
-  </si>
-  <si>
-    <t xml:space="preserve">data label fonts are controlled by standard font attributes with the prefix "heatmap_"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Various</t>
+    <t xml:space="preserve">heatmap_edge_width</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Width of the edges of the heat map cells</t>
+  </si>
+  <si>
+    <t xml:space="preserve">heatmap_font_color</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hex color string for the value label text</t>
+  </si>
+  <si>
+    <t xml:space="preserve">heatmap_font_size</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Font size of the value label text</t>
+  </si>
+  <si>
+    <t xml:space="preserve">heatmap_interp | interp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">imshow interpolation scheme (see https://matplotlib.org/stable/gallery/images_contours_and_fields/interpolation_methods.html)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">'none’</t>
   </si>
   <si>
     <t xml:space="preserve">conf_int</t>
@@ -2089,17 +2048,17 @@
       <family val="0"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="10"/>
       <color rgb="FF333333"/>
       <name val="Courier New"/>
       <family val="3"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -2144,7 +2103,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2205,8 +2164,12 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -7783,7 +7746,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
+      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8247,8 +8210,8 @@
   </sheetPr>
   <dimension ref="A1:E1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E12" activeCellId="0" sqref="E12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8806,10 +8769,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8855,18 +8818,18 @@
         <v>537</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>457</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>59</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" s="16" t="s">
         <v>538</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>104</v>
+        <v>459</v>
       </c>
       <c r="E3" s="14" t="s">
         <v>539</v>
@@ -8889,24 +8852,78 @@
         <v>542</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
         <v>543</v>
       </c>
       <c r="B5" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="0" t="s">
         <v>544</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="D5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" s="14" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
         <v>545</v>
       </c>
-      <c r="D5" s="0" t="s">
+      <c r="B6" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="0" t="s">
         <v>546</v>
       </c>
-      <c r="E5" s="14" t="s">
+      <c r="D6" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>547</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>548</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>549</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="16" t="s">
+        <v>550</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>551</v>
+      </c>
+      <c r="E8" s="0" t="s">
         <v>69</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C8" r:id="rId1" display="https://matplotlib.org/stable/gallery/images_contours_and_fields/interpolation_methods.html"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -8952,53 +8969,53 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>547</v>
+        <v>552</v>
       </c>
       <c r="B2" s="0" t="s">
         <v>21</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>548</v>
+        <v>553</v>
       </c>
       <c r="D2" s="0" t="s">
         <v>69</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>549</v>
+        <v>554</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>550</v>
+        <v>555</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>9</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>551</v>
+        <v>556</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>69</v>
       </c>
       <c r="E3" s="14" t="s">
-        <v>552</v>
+        <v>557</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>553</v>
+        <v>558</v>
       </c>
       <c r="B4" s="0" t="s">
         <v>9</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>554</v>
+        <v>559</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>69</v>
       </c>
       <c r="E4" s="14" t="s">
-        <v>552</v>
+        <v>557</v>
       </c>
     </row>
   </sheetData>
@@ -9051,30 +9068,30 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>555</v>
+        <v>560</v>
       </c>
       <c r="B2" s="0" t="s">
         <v>59</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>556</v>
+        <v>561</v>
       </c>
       <c r="D2" s="14" t="s">
         <v>93</v>
       </c>
       <c r="E2" s="14" t="s">
-        <v>557</v>
+        <v>562</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>558</v>
+        <v>563</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>59</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>559</v>
+        <v>564</v>
       </c>
       <c r="D3" s="14" t="s">
         <v>93</v>
@@ -9085,13 +9102,13 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>560</v>
+        <v>565</v>
       </c>
       <c r="B4" s="0" t="s">
         <v>59</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>561</v>
+        <v>566</v>
       </c>
       <c r="D4" s="14" t="s">
         <v>104</v>
@@ -9102,13 +9119,13 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>562</v>
+        <v>567</v>
       </c>
       <c r="B5" s="0" t="s">
         <v>59</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>563</v>
+        <v>568</v>
       </c>
       <c r="D5" s="14" t="s">
         <v>93</v>
@@ -9119,13 +9136,13 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>564</v>
+        <v>569</v>
       </c>
       <c r="B6" s="0" t="s">
         <v>59</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>565</v>
+        <v>570</v>
       </c>
       <c r="D6" s="14" t="s">
         <v>104</v>
@@ -9136,30 +9153,30 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>566</v>
+        <v>571</v>
       </c>
       <c r="B7" s="0" t="s">
         <v>59</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>567</v>
+        <v>572</v>
       </c>
       <c r="D7" s="14" t="s">
         <v>104</v>
       </c>
       <c r="E7" s="14" t="s">
-        <v>568</v>
+        <v>573</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>569</v>
+        <v>574</v>
       </c>
       <c r="B8" s="0" t="s">
         <v>59</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>570</v>
+        <v>575</v>
       </c>
       <c r="D8" s="14" t="s">
         <v>104</v>
@@ -9170,13 +9187,13 @@
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>571</v>
+        <v>576</v>
       </c>
       <c r="B9" s="0" t="s">
         <v>59</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>572</v>
+        <v>577</v>
       </c>
       <c r="D9" s="14" t="s">
         <v>104</v>
@@ -9187,13 +9204,13 @@
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>573</v>
+        <v>578</v>
       </c>
       <c r="B10" s="0" t="s">
         <v>59</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>574</v>
+        <v>579</v>
       </c>
       <c r="D10" s="14" t="s">
         <v>104</v>
@@ -9204,13 +9221,13 @@
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>575</v>
+        <v>580</v>
       </c>
       <c r="B11" s="0" t="s">
         <v>59</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>576</v>
+        <v>581</v>
       </c>
       <c r="D11" s="14" t="s">
         <v>104</v>
@@ -9221,13 +9238,13 @@
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>577</v>
+        <v>582</v>
       </c>
       <c r="B12" s="0" t="s">
         <v>9</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>578</v>
+        <v>583</v>
       </c>
       <c r="D12" s="14" t="s">
         <v>26</v>
@@ -9238,13 +9255,13 @@
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>579</v>
+        <v>584</v>
       </c>
       <c r="B13" s="0" t="s">
         <v>9</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>580</v>
+        <v>585</v>
       </c>
       <c r="D13" s="14" t="s">
         <v>55</v>
@@ -9255,13 +9272,13 @@
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>581</v>
+        <v>586</v>
       </c>
       <c r="B14" s="0" t="s">
         <v>21</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>582</v>
+        <v>587</v>
       </c>
       <c r="D14" s="0" t="n">
         <v>1.3</v>
@@ -9317,135 +9334,135 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>583</v>
+        <v>588</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>93</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>584</v>
+        <v>589</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>93</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>585</v>
+        <v>590</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="0" t="s">
-        <v>586</v>
+        <v>591</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>587</v>
+        <v>592</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>588</v>
+        <v>593</v>
       </c>
       <c r="D4" s="0" t="s">
         <v>69</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>589</v>
+        <v>594</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>590</v>
+        <v>595</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>591</v>
+        <v>596</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>592</v>
+        <v>597</v>
       </c>
       <c r="D5" s="0" t="s">
         <v>69</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>593</v>
+        <v>598</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>594</v>
+        <v>599</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>595</v>
+        <v>600</v>
       </c>
       <c r="D6" s="0" t="s">
         <v>69</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>596</v>
+        <v>601</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>597</v>
+        <v>602</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>71</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>598</v>
+        <v>603</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>599</v>
+        <v>604</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>600</v>
+        <v>605</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>601</v>
+        <v>606</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>602</v>
+        <v>607</v>
       </c>
       <c r="D8" s="0" t="s">
         <v>69</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>603</v>
+        <v>608</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>604</v>
+        <v>609</v>
       </c>
       <c r="B9" s="0" t="s">
         <v>59</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>605</v>
+        <v>610</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>93</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>606</v>
+        <v>611</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>607</v>
+        <v>612</v>
       </c>
       <c r="B10" s="0" t="s">
         <v>59</v>
@@ -9460,13 +9477,13 @@
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>608</v>
+        <v>613</v>
       </c>
       <c r="B11" s="0" t="s">
         <v>59</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>609</v>
+        <v>614</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>93</v>
@@ -9475,13 +9492,13 @@
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>610</v>
+        <v>615</v>
       </c>
       <c r="B12" s="0" t="s">
         <v>59</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>611</v>
+        <v>616</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>93</v>
@@ -9490,13 +9507,13 @@
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>612</v>
+        <v>617</v>
       </c>
       <c r="B13" s="0" t="s">
         <v>59</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>613</v>
+        <v>618</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>93</v>
@@ -9505,13 +9522,13 @@
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>614</v>
+        <v>619</v>
       </c>
       <c r="B14" s="0" t="s">
         <v>59</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>615</v>
+        <v>620</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>104</v>
@@ -9520,13 +9537,13 @@
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>616</v>
+        <v>621</v>
       </c>
       <c r="B15" s="0" t="s">
         <v>59</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>617</v>
+        <v>622</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>104</v>
@@ -9535,13 +9552,13 @@
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>618</v>
+        <v>623</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>619</v>
+        <v>624</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>620</v>
+        <v>625</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>69</v>
@@ -9554,7 +9571,7 @@
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="0" t="s">
-        <v>621</v>
+        <v>626</v>
       </c>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
@@ -9563,20 +9580,20 @@
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="3" t="s">
-        <v>622</v>
+        <v>627</v>
       </c>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>623</v>
+        <v>628</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>619</v>
+        <v>624</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>624</v>
+        <v>629</v>
       </c>
       <c r="D19" s="4" t="s">
         <v>69</v>
@@ -9587,13 +9604,13 @@
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>625</v>
+        <v>630</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>619</v>
+        <v>624</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>624</v>
+        <v>629</v>
       </c>
       <c r="D20" s="4" t="s">
         <v>69</v>
@@ -9604,13 +9621,13 @@
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>626</v>
+        <v>631</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>619</v>
+        <v>624</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>624</v>
+        <v>629</v>
       </c>
       <c r="D21" s="4" t="s">
         <v>69</v>
@@ -9621,13 +9638,13 @@
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>627</v>
+        <v>632</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>619</v>
+        <v>624</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>624</v>
+        <v>629</v>
       </c>
       <c r="D22" s="4" t="s">
         <v>69</v>
@@ -9638,16 +9655,16 @@
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>628</v>
+        <v>633</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>629</v>
+        <v>634</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>630</v>
+        <v>635</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>631</v>
+        <v>636</v>
       </c>
     </row>
   </sheetData>
@@ -9705,41 +9722,41 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>632</v>
+        <v>637</v>
       </c>
       <c r="B2" s="0" t="s">
         <v>9</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>633</v>
+        <v>638</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>634</v>
+        <v>639</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>635</v>
+        <v>640</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>9</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>636</v>
+        <v>641</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>637</v>
+        <v>642</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>638</v>
+        <v>643</v>
       </c>
       <c r="B4" s="0" t="s">
         <v>59</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>639</v>
+        <v>644</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>93</v>
@@ -9747,13 +9764,13 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>640</v>
+        <v>645</v>
       </c>
       <c r="B5" s="0" t="s">
         <v>59</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>641</v>
+        <v>646</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>104</v>
@@ -9761,13 +9778,13 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>642</v>
+        <v>647</v>
       </c>
       <c r="B6" s="0" t="s">
         <v>59</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>643</v>
+        <v>648</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>104</v>
@@ -9775,13 +9792,13 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>644</v>
+        <v>649</v>
       </c>
       <c r="B7" s="0" t="s">
         <v>59</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>645</v>
+        <v>650</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>93</v>
@@ -9789,27 +9806,27 @@
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>646</v>
+        <v>651</v>
       </c>
       <c r="B8" s="0" t="s">
         <v>9</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>647</v>
+        <v>652</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>648</v>
+        <v>653</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>649</v>
+        <v>654</v>
       </c>
       <c r="B9" s="0" t="s">
         <v>59</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>650</v>
+        <v>655</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>104</v>

</xml_diff>